<commit_message>
Added options for single trial plot
</commit_message>
<xml_diff>
--- a/layout.xlsx
+++ b/layout.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="50" windowWidth="13380" windowHeight="4580"/>
+    <workbookView xWindow="400" yWindow="50" windowWidth="13380" windowHeight="4580" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Main window" sheetId="1" r:id="rId1"/>
+    <sheet name="f3-single trial" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>f2-ttk.Frame (session viewer)</t>
   </si>
@@ -64,6 +64,27 @@
   </si>
   <si>
     <t>onsetMenu - ttk.OptionMenu</t>
+  </si>
+  <si>
+    <t>alltrialsMenu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shownoiseLbl </t>
+  </si>
+  <si>
+    <t>shownoiseCheckbutton</t>
+  </si>
+  <si>
+    <t>trialEntry</t>
+  </si>
+  <si>
+    <t>prevBtn</t>
+  </si>
+  <si>
+    <t>nextBtn</t>
+  </si>
+  <si>
+    <t>Figure</t>
   </si>
 </sst>
 </file>
@@ -220,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -229,47 +250,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,7 +598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6:K6"/>
     </sheetView>
   </sheetViews>
@@ -623,16 +647,16 @@
         <v>10</v>
       </c>
       <c r="C2" s="1"/>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" spans="1:11" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3">
@@ -641,14 +665,14 @@
       <c r="B3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="14"/>
     </row>
     <row r="4" spans="1:11" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4">
@@ -657,14 +681,14 @@
       <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="17"/>
     </row>
     <row r="5" spans="1:11" ht="33.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5">
@@ -688,35 +712,35 @@
       <c r="G5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I5" s="17" t="s">
+      <c r="I5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K5" s="6"/>
+      <c r="K5" s="8"/>
     </row>
     <row r="6" spans="1:11" ht="114" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4" t="s">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A7">
@@ -750,12 +774,113 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="4" width="17.54296875" customWidth="1"/>
+    <col min="5" max="5" width="50.7265625" customWidth="1"/>
+    <col min="6" max="10" width="17.54296875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1">
+        <v>6</v>
+      </c>
+      <c r="I1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="18"/>
+    </row>
+    <row r="4" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="18"/>
+    </row>
+    <row r="5" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="E5" s="18"/>
+    </row>
+    <row r="6" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E2:E5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added (non-functional) progress bar
</commit_message>
<xml_diff>
--- a/layout.xlsx
+++ b/layout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="400" yWindow="50" windowWidth="13380" windowHeight="4580" activeTab="1"/>
+    <workbookView xWindow="400" yWindow="50" windowWidth="13380" windowHeight="4580"/>
   </bookViews>
   <sheets>
     <sheet name="Main window" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>f2-ttk.Frame (session viewer)</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Figure</t>
+  </si>
+  <si>
+    <t>View session - ttk.Button</t>
+  </si>
+  <si>
+    <t>bluesig-menu</t>
+  </si>
+  <si>
+    <t>uvsig-menu</t>
   </si>
 </sst>
 </file>
@@ -598,8 +607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6:K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -646,7 +655,9 @@
       <c r="B2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D2" s="9" t="s">
         <v>0</v>
       </c>
@@ -664,6 +675,9 @@
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="13"/>
@@ -680,6 +694,9 @@
       </c>
       <c r="B4" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="16"/>
@@ -776,7 +793,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed naming of lick runs
</commit_message>
<xml_diff>
--- a/layout.xlsx
+++ b/layout.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>f2-ttk.Frame (session viewer)</t>
   </si>
@@ -107,9 +107,6 @@
     <t>noisethField - ttk.Entry</t>
   </si>
   <si>
-    <t>noiseBtn - ttk.Button</t>
-  </si>
-  <si>
     <t>trialField - ttk.Entry</t>
   </si>
   <si>
@@ -137,10 +134,19 @@
     <t>makelickrunsBtn - ttk.Button</t>
   </si>
   <si>
-    <t>lickrunsLbl - ttk.Label</t>
-  </si>
-  <si>
     <t>f3-ttk.Frame (processed)</t>
+  </si>
+  <si>
+    <t>choosestreamMenu - ttk.OptionMenu</t>
+  </si>
+  <si>
+    <t>lickrunseventMenu - ttk.OptionMenu</t>
+  </si>
+  <si>
+    <t>noiseBtn - ttk.RadioButton</t>
+  </si>
+  <si>
+    <t>noisethLbl - ttk.Label</t>
   </si>
 </sst>
 </file>
@@ -284,58 +290,88 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,7 +680,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="J6" sqref="J6:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,291 +689,293 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12">
+      <c r="A1" s="5"/>
+      <c r="B1" s="5">
         <v>0</v>
       </c>
-      <c r="C1" s="12">
+      <c r="C1" s="5">
         <v>1</v>
       </c>
-      <c r="D1" s="12">
+      <c r="D1" s="5">
         <v>2</v>
       </c>
-      <c r="E1" s="12">
+      <c r="E1" s="5">
         <v>3</v>
       </c>
-      <c r="F1" s="12">
+      <c r="F1" s="5">
         <v>4</v>
       </c>
-      <c r="G1" s="12">
+      <c r="G1" s="5">
         <v>5</v>
       </c>
-      <c r="H1" s="12">
+      <c r="H1" s="5">
         <v>6</v>
       </c>
-      <c r="I1" s="12">
+      <c r="I1" s="5">
         <v>7</v>
       </c>
-      <c r="J1" s="12">
+      <c r="J1" s="5">
         <v>8</v>
       </c>
-      <c r="K1" s="12">
+      <c r="K1" s="5">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
+      <c r="A2" s="5">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="3" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="K2" s="15"/>
+    </row>
+    <row r="3" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="K3" s="18"/>
+    </row>
+    <row r="4" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="K4" s="21"/>
+    </row>
+    <row r="5" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>4</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="15"/>
-    </row>
-    <row r="3" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12">
+      <c r="C6" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="16"/>
-    </row>
-    <row r="4" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12">
+      <c r="E6" s="23"/>
+      <c r="F6" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="23"/>
+      <c r="H6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="I6" s="25"/>
+      <c r="J6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>5</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="26"/>
+      <c r="J7" s="9"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>6</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="26"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>7</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="26"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>8</v>
       </c>
-      <c r="C4" s="1"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="17"/>
-    </row>
-    <row r="5" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12">
-        <v>3</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="12">
-        <v>4</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="12">
-        <v>5</v>
-      </c>
-      <c r="B7" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="1" t="s">
+      <c r="B10" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="12">
-        <v>6</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="1"/>
-    </row>
-    <row r="9" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="12">
-        <v>7</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="F11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="1"/>
-    </row>
-    <row r="10" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12">
-        <v>8</v>
-      </c>
-      <c r="B10" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="1"/>
-    </row>
-    <row r="11" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="12">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="1" t="s">
+      <c r="E12" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G12" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-    </row>
-    <row r="12" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="12">
-        <v>10</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="G12" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="13"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="13"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
     </row>
     <row r="13" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="H6:I10"/>
+    <mergeCell ref="J6:K7"/>
     <mergeCell ref="D6:E10"/>
     <mergeCell ref="F6:G10"/>
-    <mergeCell ref="H6:J10"/>
     <mergeCell ref="D2:F4"/>
-    <mergeCell ref="H2:J4"/>
+    <mergeCell ref="G2:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -992,7 +1030,7 @@
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1009,7 +1047,7 @@
       <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1021,13 +1059,13 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">

</xml_diff>

<commit_message>
updated and made functioning .exe
</commit_message>
<xml_diff>
--- a/layout.xlsx
+++ b/layout.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>f2-ttk.Frame (session viewer)</t>
   </si>
@@ -101,9 +101,6 @@
     <t>f5-ttk.Frame(heat map)</t>
   </si>
   <si>
-    <t>noiseLbl - ttk.Label</t>
-  </si>
-  <si>
     <t>noisethField - ttk.Entry</t>
   </si>
   <si>
@@ -143,20 +140,33 @@
     <t>lickrunseventMenu - ttk.OptionMenu</t>
   </si>
   <si>
-    <t>noiseBtn - ttk.RadioButton</t>
-  </si>
-  <si>
     <t>noisethLbl - ttk.Label</t>
+  </si>
+  <si>
+    <t>refreshBtn - ttk.Button</t>
+  </si>
+  <si>
+    <t>noiseBtn - ttk.Button</t>
+  </si>
+  <si>
+    <t>progress bar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -170,7 +180,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -201,16 +211,9 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
+      <bottom style="thin">
         <color indexed="64"/>
-      </top>
-      <bottom/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -221,94 +224,44 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -316,61 +269,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -677,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6:K7"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -689,40 +591,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5"/>
-      <c r="B1" s="5">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1">
         <v>0</v>
       </c>
-      <c r="C1" s="5">
+      <c r="C1" s="1">
         <v>1</v>
       </c>
-      <c r="D1" s="5">
+      <c r="D1" s="1">
         <v>2</v>
       </c>
-      <c r="E1" s="5">
+      <c r="E1" s="1">
         <v>3</v>
       </c>
-      <c r="F1" s="5">
+      <c r="F1" s="1">
         <v>4</v>
       </c>
-      <c r="G1" s="5">
+      <c r="G1" s="1">
         <v>5</v>
       </c>
-      <c r="H1" s="5">
+      <c r="H1" s="1">
         <v>6</v>
       </c>
-      <c r="I1" s="5">
+      <c r="I1" s="1">
         <v>7</v>
       </c>
-      <c r="J1" s="5">
+      <c r="J1" s="1">
         <v>8</v>
       </c>
-      <c r="K1" s="5">
+      <c r="K1" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -731,20 +633,21 @@
       <c r="C2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="K2" s="15"/>
+        <v>36</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -753,38 +656,40 @@
       <c r="C3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="K3" s="18"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="4"/>
     </row>
     <row r="4" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="K4" s="21"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="4"/>
     </row>
     <row r="5" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="4"/>
@@ -797,34 +702,34 @@
       <c r="K5" s="4"/>
     </row>
     <row r="6" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="D6" s="23" t="s">
+      <c r="B6" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23" t="s">
+      <c r="E6" s="5"/>
+      <c r="F6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="G6" s="23"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="25"/>
+      <c r="I6" s="7"/>
       <c r="J6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K6" s="8"/>
+      <c r="K6" s="7"/>
     </row>
     <row r="7" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -833,17 +738,17 @@
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="10"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
     </row>
     <row r="8" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -852,19 +757,19 @@
       <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="6" t="s">
-        <v>38</v>
-      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="J8" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" s="14"/>
     </row>
     <row r="9" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -873,93 +778,93 @@
       <c r="C9" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="4" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+    </row>
+    <row r="10" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>8</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="4" t="s">
-        <v>40</v>
-      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="8"/>
     </row>
     <row r="11" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+        <v>33</v>
+      </c>
+      <c r="H11" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>40</v>
+      </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
     </row>
     <row r="12" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24" t="s">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E12" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
+      <c r="F12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
@@ -968,14 +873,35 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>12</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="10">
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B4:C4"/>
     <mergeCell ref="H6:I10"/>
     <mergeCell ref="J6:K7"/>
     <mergeCell ref="D6:E10"/>
     <mergeCell ref="F6:G10"/>
     <mergeCell ref="D2:F4"/>
     <mergeCell ref="G2:I4"/>
+    <mergeCell ref="J8:K9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1030,7 +956,7 @@
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="6" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1047,7 +973,7 @@
       <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="6"/>
     </row>
     <row r="4" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1059,13 +985,13 @@
       <c r="C4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="6"/>
     </row>
     <row r="5" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6">

</xml_diff>